<commit_message>
auto eval for accuracy added
</commit_message>
<xml_diff>
--- a/Results/50ques_results_bing - Copy/query_llama2.xlsx
+++ b/Results/50ques_results_bing - Copy/query_llama2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAMES_SETUP\Thesis\Code\Results\50ques_results_bing - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5916D9-6BE5-4819-9781-48DECEDA4EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33108E70-DC02-4347-ADB5-E4BBB26A1C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{138B884C-2B9A-4C3A-A489-4514957348AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="417">
   <si>
     <t>ques_id</t>
   </si>
@@ -878,18 +878,9 @@
     <t>Harry Maguire has never won the Ballon d'Or.</t>
   </si>
   <si>
-    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center-back for Premier League club Manchester United and the England national team. He has been named in the PFA Team of the Year twice and has won the UEFA Nations League with England. However, he has not won the Ballon d'Or award.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': "Wikipedia - Ballon d'Or", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "InvalidExplanation: The question asks about the first year in which Harry Maguire won the Ballon d'Or, but Harry Maguire has never won the Ballon d'Or award. Therefore, the premise of the question is invalid."}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center-back for Manchester United and the England national team. He has been named in the PFA Team of the Year twice and has won the UEFA Nations League with England. However, he has not won the Ballon d'Or award.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': "Wikipedia - Ballon d'Or", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "InvalidExplanation: The question asks about the first year in which Harry Maguire won the Ballon d'Or, but Harry Maguire has never won the Ballon d'Or award. Therefore, the premise of the question is invalid.Note: The question is based on a false assumption that Harry Maguire has won the Ballon d'Or award, which is not true.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
     <t>{'webPages': [{'name': "The full list of Ballon d'Or winners - from 1956 to the present day", 'url': 'https://inews.co.uk/sport/football/ballon-dor-winners-full-list-history-206332', 'snippet': "Sport Football Tables Latest Ballon dâ€™Or: Full list of winners, from 1956 to the present day as Lionel Messi wins 2023 award The award is widely seen as the most prestigious in football's..."}, {'name': "List of the Ballon d'Or Winners - Topend Sports", 'url': 'https://www.topendsports.com/sport/soccer/list-player-of-the-year-ballondor.htm', 'snippet': "2023 Award The 30 nominees for the 2023 Ballon d'Or award were announced in September 2023. Lionel Messi was included on the list after being left off in 2022, and was annouced as the winner of his 8th Ballon d'Or on October 30. List of Men's Ballon d'Or award winners Related Pages Ballon d'Or Home Women's Ballon d'Or award"}], 'entities': [{'name': "Ballon d'Or", 'url': 'https://en.wikipedia.org/wiki/Ballon_d%27Or', 'snippet': "The Ballon d'Or is an annual football award presented by French news magazine France Football since 1956 and co-organized alongside UEFA since 2024. Between 2010 and 2015, in an agreement with FIFA, the award was temporarily merged with the FIFA World Player of the Year and known as the FIFA Ballon d'Or. That partnership ended in 2016, and the award reverted to the Ballon d'Or, while FIFA also reverted to its own separate annual award The Best FIFA Men's Player. The recipients of the joint FIFA Ballon d'Or are considered as winners by both award organisations."}]}</t>
   </si>
   <si>
-    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center-back for Manchester United and the England national team. He has been named in the PFA Team of the Year twice and has won the UEFA Nations League with England. However, he has not won the Ballon d'Or award.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': "Wikipedia - Ballon d'Or", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "InvalidExplanation: The question asks about the first year in which Harry Maguire won the Ballon d'Or, but Harry Maguire has never won the Ballon d'Or award. Therefore, the premise of the question is invalid.Note: The question is based on a false assumption that Harry Maguire has won the Ballon d'Or award, which is not true.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
     <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center-back for Premier League club Manchester United and the England national team. He has been named in the PFA Team of the Year twice and has won the UEFA Nations League with England. However, he has not won the Ballon d'Or award.", 'Answer:': "Harry Maguire has never won the Ballon d'Or.", 'Confidence Level:': '100%', 'Source:': "Wikipedia - Ballon d'Or", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "InvalidExplanation: The premise of the question is invalid because Harry Maguire has never won the Ballon d'Or award. The question asks for the first year in which Harry Maguire won the Ballon d'Or, but since he has never won it, there is no correct answer.Note: The confidence level of 100% indicates that I am certain that Harry Maguire has never won the Ballon d'Or, based on my knowledge and information available on Wikipedia. The source reference is provided for further verification. The core concept of the question is Ballon d'Or, which is the award in question. The premise of the question is invalid because it asks for information that does not exist.", 'Certainty_Estimation': 'Yes'}</t>
   </si>
   <si>
@@ -1272,6 +1263,30 @@
   </si>
   <si>
     <t>{'Explanation:': 'The FIFA World Cup is an international soccer tournament held every four years, where national teams compete to win the championship. The location of the tournament changes each year, and the host country or countries are selected through a bidding process.', 'Answer:': 'The FIFA World Cup will be hosted in the United States, Mexico, and Canada in 2026.', 'Confidence Level:': '90%', 'Source:': 'FIFA.com (Official FIFA website)', 'Core Concept:': 'FIFA World Cup, host country', 'Premise of the Question:': 'ValidExplanation: The premise of the question is valid because it is based on the fact that the FIFA World Cup is a recurring event that takes place every four years, and the location changes each year. The question is asking for the location of the next FIFA World Cup, which is a valid and relevant question.Source:* FIFA.com (Official FIFA website) - This is the official website of FIFA, the governing body of international soccer. It provides information on the FIFA World Cup, including the location of upcoming tournaments.Core Concept:* FIFA World Cup - This is the main concept related to the question. It refers to the international soccer tournament that takes place every four years.* Host country - This is the secondary concept related to the question. It refers to the country or countries that host the FIFA World Cup.Premise of the Question:* Valid - The premise of the question is valid because it is based on a factual event that takes place regularly, and the information requested is relevant to the event.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center back for Manchester United and the England national team. He has been named in the PFA Team of the Year three times and has won the Manchester United Player of the Year award twice. However, he has not won the Ballon d'Or award in any year.", 'Answer:': "No, Harry Maguire has not won the Ballon d'Or in any year.", 'Confidence Level:': '90%', 'Source:': "Harry Maguire - Wikipedia, Ballon d'Or Winners (1956 - 2021) [Complete List]", 'Core Concept:': "Ballon d'Or, Harry Maguire", 'Premise of the Question:': "ValidThe premise of the question is valid because it asks whether Harry Maguire has won the Ballon d'Or in any year, which is a factual question that can be answered by looking at the list of Ballon d'Or winners. The question does not contain any false or misleading information, and it is not trying to trick the agent into giving an incorrect answer. Therefore, the premise of the question is valid."}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center back for Manchester United and the England national team. He has been named the club's Player of the Year three seasons in a row and has also won the Premier League with Manchester United. However, the question asks if he has won the Ballon d'Or in any year, which is an annual football award presented by French news magazine France Football since 1956.", 'Answer:': "No, Harry Maguire has not won the Ballon d'Or in any year.", 'Confidence Level:': '100.0%', 'Source:': "Ballon d'Or Winners (1956 - 2021) [Complete List] - Soccerwhizz.com", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "ValidThe question is asking about Harry Maguire's achievements and whether he has won the Ballon d'Or in any year. The premise of the question is valid as it is based on factual information about Harry Maguire's career and the Ballon d'Or award. The question does not contain any false assumptions or misinformation, and it is a legitimate question that can be answered with factual data.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'webPages': [{'name': "The full list of Ballon d'Or winners - from 1956 to the present day", 'url': 'https://inews.co.uk/sport/football/ballon-dor-winners-full-list-history-206332', 'snippet': 'The award was then opened to players in any league across the world in 2007 before being merged with the rival Fifa Player of the Year in 2010. The two trophies went their separate ways again...'}, {'name': "List of the Ballon d'Or Winners - Topend Sports", 'url': 'https://www.topendsports.com/sport/soccer/list-player-of-the-year-ballondor.htm', 'snippet': "The Ballon d'Or award is an annual football award for the best player over the previous year. It was first awarded in 1956. The most recent winner was Argentinan Lionel Messi in 2023. Messi has won the men's Ballon d'Or award a record eight times, Cristiano Ronaldo has won the award five times."}, {'name': 'Harry Maguire - Wikipedia', 'url': 'https://en.wikipedia.org/wiki/Harry_Maguire', 'snippet': "Jacob Harry Maguire (born 5 March 1993) is an English professional footballer who plays as a centre back for Premier League club Manchester United and the England national team.. Maguire came through the youth system at Sheffield United before graduating to the first team in 2011. He made 166 appearances for United and was the club's Player of the Year three seasons in succession, also ..."}, {'name': 'Harry Maguire - Titles &amp; achievements | Transfermarkt', 'url': 'https://www.transfermarkt.com/harry-maguire/erfolge/spieler/177907', 'snippet': '1 Man Utd Premier League League level: First Tier Joined: Aug 5, 2019 Contract expires: Jun 30, 2025 IMAGO + Date of birth/Age: Mar 5, 1993 (30) Place of birth: Sheffield Citizenship: England Height: 1,94 m Position: Centre-Back Current international: England Caps/Goals: 62 / 7 € 20.00 m Last update: Dec 19, 2023 Profile Stats Market value'}, {'name': "Ballon d'Or Winners (1956 - 2021) [Complete List]", 'url': 'https://soccerwhizz.com/ballon-dor-winners/', 'snippet': 'He collected the record-breaking seventh in the 2021 campaign, coming ahead of other great players in the vote like Bayern Munich’s Robert Lewandowski and Chelsea’s Jorginho.'}], 'entities': [{'name': "Ballon d'Or", 'url': 'https://en.wikipedia.org/wiki/Ballon_d%27Or', 'snippet': "The Ballon d'Or is an annual football award presented by French news magazine France Football since 1956 and co-organized alongside UEFA since 2024. Between 2010 and 2015, in an agreement with FIFA, the award was temporarily merged with the FIFA World Player of the Year and known as the FIFA Ballon d'Or. That partnership ended in 2016, and the award reverted to the Ballon d'Or, while FIFA also reverted to its own separate annual award The Best FIFA Men's Player. The recipients of the joint FIFA Ballon d'Or are considered as winners by both award organisations."}]}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center back for Manchester United and the England national team. He has been named the club's Player of the Year three seasons in a row and has also won the Premier League with Manchester United. However, the question asks if he has won the Ballon d'Or in any year, which is an annual football award presented by French news magazine France Football since 1956.", 'Answer:': "No, Harry Maguire has not won the Ballon d'Or in any year.", 'Confidence Level:': '80%', 'Source:': "Ballon d'Or Winners (1956 - 2021) [Complete List] - Soccerwhizz.com", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "ValidThe question is asking about Harry Maguire's achievements and whether he has won the Ballon d'Or in any year. The premise of the question is valid as it is based on factual information about Harry Maguire's career and the Ballon d'Or award. The question does not contain any false assumptions or misinformation, and it is a legitimate question that can be answered with factual data.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center back for Manchester United and the England national team. He has been named the Player of the Year for his club and has also received caps for his country, but has he won the prestigious Ballon d'Or award?", 'Answer:': "No, Harry Maguire has not won the Ballon d'Or award in any year.", 'Confidence Level:': '80%', 'Source:': "Ballon d'Or Winners (1956 - 2021) [Complete List] (&lt;https://soccerwhizz.com/ballon-dor-winners/&gt;)", 'Core Concept:': "Ballon d'Or winners", 'Premise of the Question:': "ValidThe question is asking about whether Harry Maguire has won the Ballon d'Or award, which is a valid question as the award is given annually to the best football player in the world. The question provides enough information to answer it, and the answer can be found by checking the list of Ballon d'Or winners.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Harry Maguire has been an English professional footballer who plays as a center-back for Manchester United and the England national team. He has been named in the PFA Team of the Year twice ", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': "Wikipedia - Ballon d'Or", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "InvalidExplanation: The question asks about the first year in which Harry Maguire won the Ballon d'Or, but Harry Maguire has never won the Ballon d'Or award. Therefore, the premise of the question is invalid.Note: The question is based on a false assumption that Harry Maguire has won the Ballon d'Or award, which is not true.", 'Certainty_Estimation': 'No'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Harry Maguire is an English professional footballer who plays as a center-back for Manchester United and the England national team. He has been named in the PFA Team of the Year twice and has won the UEFA Nations League with England.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': "Wikipedia - Ballon d'Or", 'Core Concept:': "Ballon d'Or", 'Premise of the Question:': "InvalidExplanation: The question asks about the first year in which Harry Maguire won the Ballon d'Or, but Harry Maguire has never won the Ballon d'Or award. Therefore, the premise of the question is invalid.Note: The question is based on a false assumption that Harry Maguire has won the Ballon d'Or award, which is not true.", 'Certainty_Estimation': 'No'}</t>
+  </si>
+  <si>
+    <t>Harry Maguire AND year AND won the Ballon d'Or</t>
   </si>
 </sst>
 </file>
@@ -1673,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36871A47-521C-4433-BA8A-E7C6A1C714C6}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63:I63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2251,10 +2266,10 @@
         <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G18">
         <v>100</v>
@@ -2263,10 +2278,10 @@
         <v>126</v>
       </c>
       <c r="I18" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J18" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -3005,19 +3020,19 @@
         <v>274</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41" t="s">
         <v>406</v>
       </c>
-      <c r="G41">
-        <v>100</v>
-      </c>
-      <c r="H41" t="s">
-        <v>409</v>
-      </c>
       <c r="I41" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="J41" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -3034,354 +3049,357 @@
         <v>279</v>
       </c>
       <c r="E42" t="s">
+        <v>281</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" t="s">
+        <v>100</v>
+      </c>
+      <c r="H42" t="s">
         <v>280</v>
       </c>
-      <c r="F42" t="s">
+      <c r="I42" t="s">
+        <v>415</v>
+      </c>
+      <c r="J42" t="s">
         <v>281</v>
       </c>
-      <c r="G42">
-        <v>100</v>
-      </c>
-      <c r="H42" t="s">
-        <v>282</v>
-      </c>
-      <c r="I42" t="s">
-        <v>283</v>
-      </c>
-      <c r="J42" t="s">
-        <v>284</v>
+      <c r="K42" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>285</v>
+        <v>416</v>
       </c>
       <c r="D43" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E43" t="s">
-        <v>287</v>
-      </c>
-      <c r="F43" t="s">
-        <v>288</v>
+        <v>409</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="G43">
         <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>289</v>
+        <v>411</v>
       </c>
       <c r="I43" t="s">
-        <v>290</v>
+        <v>412</v>
       </c>
       <c r="J43" t="s">
-        <v>291</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D44" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="E44" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F44" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="G44">
-        <v>65.52</v>
+        <v>100</v>
       </c>
       <c r="H44" t="s">
+        <v>286</v>
+      </c>
+      <c r="I44" t="s">
+        <v>287</v>
+      </c>
+      <c r="J44" t="s">
+        <v>288</v>
+      </c>
+      <c r="K44" t="s">
         <v>296</v>
-      </c>
-      <c r="I44" t="s">
-        <v>297</v>
-      </c>
-      <c r="J44" t="s">
-        <v>298</v>
-      </c>
-      <c r="K44" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="D45" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="E45" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="F45" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="G45">
-        <v>100</v>
+        <v>65.52</v>
       </c>
       <c r="H45" t="s">
+        <v>293</v>
+      </c>
+      <c r="I45" t="s">
+        <v>294</v>
+      </c>
+      <c r="J45" t="s">
+        <v>295</v>
+      </c>
+      <c r="K45" t="s">
         <v>304</v>
-      </c>
-      <c r="I45" t="s">
-        <v>305</v>
-      </c>
-      <c r="J45" t="s">
-        <v>306</v>
-      </c>
-      <c r="K45" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D46" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E46" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F46" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="G46">
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="I46" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="J46" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="D47" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E47" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F47" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="G47">
         <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="I47" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="J47" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D48" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E48" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="F48" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="G48">
         <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="I48" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="J48" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D49" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="E49" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="F49" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="G49">
         <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="I49" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="J49" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D50" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E50" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="F50" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G50">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="H50" t="s">
+        <v>330</v>
+      </c>
+      <c r="I50" t="s">
+        <v>331</v>
+      </c>
+      <c r="J50" t="s">
+        <v>332</v>
+      </c>
+      <c r="K50" t="s">
         <v>340</v>
-      </c>
-      <c r="I50" t="s">
-        <v>341</v>
-      </c>
-      <c r="J50" t="s">
-        <v>342</v>
-      </c>
-      <c r="K50" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D51" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="E51" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="F51" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="G51">
-        <v>100</v>
+        <v>66.67</v>
       </c>
       <c r="H51" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="I51" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="J51" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D52" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="E52" t="s">
-        <v>353</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G52" t="s">
+        <v>343</v>
+      </c>
+      <c r="F52" t="s">
+        <v>344</v>
+      </c>
+      <c r="G52">
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="I52" t="s">
-        <v>410</v>
+        <v>346</v>
       </c>
       <c r="J52" t="s">
-        <v>411</v>
+        <v>347</v>
       </c>
       <c r="K52" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -3389,98 +3407,98 @@
         <v>44</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D53" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E53" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G53">
+        <v>99</v>
+      </c>
+      <c r="G53" t="s">
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="I53" t="s">
-        <v>359</v>
+        <v>407</v>
       </c>
       <c r="J53" t="s">
-        <v>360</v>
+        <v>408</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D54" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="E54" t="s">
-        <v>363</v>
-      </c>
-      <c r="F54" t="s">
-        <v>364</v>
+        <v>353</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="G54">
         <v>100</v>
       </c>
       <c r="H54" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="I54" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="J54" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="D55" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E55" t="s">
-        <v>370</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G55" t="s">
+        <v>360</v>
+      </c>
+      <c r="F55" t="s">
+        <v>361</v>
+      </c>
+      <c r="G55">
         <v>100</v>
       </c>
       <c r="H55" t="s">
+        <v>362</v>
+      </c>
+      <c r="I55" t="s">
+        <v>363</v>
+      </c>
+      <c r="J55" t="s">
+        <v>364</v>
+      </c>
+      <c r="K55" t="s">
         <v>371</v>
-      </c>
-      <c r="I55" t="s">
-        <v>372</v>
-      </c>
-      <c r="J55" t="s">
-        <v>373</v>
-      </c>
-      <c r="K55" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -3488,127 +3506,159 @@
         <v>46</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D56" t="s">
+        <v>366</v>
+      </c>
+      <c r="E56" t="s">
+        <v>367</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G56" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" t="s">
+        <v>368</v>
+      </c>
+      <c r="I56" t="s">
         <v>369</v>
       </c>
-      <c r="E56" t="s">
-        <v>376</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="G56">
-        <v>100</v>
-      </c>
-      <c r="H56" t="s">
-        <v>378</v>
-      </c>
-      <c r="I56" t="s">
-        <v>379</v>
-      </c>
       <c r="J56" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D57" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="E57" t="s">
-        <v>383</v>
-      </c>
-      <c r="F57" t="s">
-        <v>384</v>
+        <v>373</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>374</v>
       </c>
       <c r="G57">
         <v>100</v>
       </c>
       <c r="H57" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="I57" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="J57" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D58" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E58" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F58" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="G58">
         <v>100</v>
       </c>
       <c r="H58" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="I58" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="J58" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
+        <v>48</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>385</v>
+      </c>
+      <c r="D59" t="s">
+        <v>386</v>
+      </c>
+      <c r="E59" t="s">
+        <v>387</v>
+      </c>
+      <c r="F59" t="s">
+        <v>388</v>
+      </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
+      <c r="H59" t="s">
+        <v>389</v>
+      </c>
+      <c r="I59" t="s">
+        <v>390</v>
+      </c>
+      <c r="J59" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>49</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>392</v>
+      </c>
+      <c r="D60" t="s">
+        <v>393</v>
+      </c>
+      <c r="E60" t="s">
+        <v>394</v>
+      </c>
+      <c r="F60" t="s">
         <v>395</v>
       </c>
-      <c r="D59" t="s">
+      <c r="G60">
+        <v>100</v>
+      </c>
+      <c r="H60" t="s">
         <v>396</v>
       </c>
-      <c r="E59" t="s">
+      <c r="I60" t="s">
         <v>397</v>
       </c>
-      <c r="F59" t="s">
+      <c r="J60" t="s">
         <v>398</v>
-      </c>
-      <c r="G59">
-        <v>100</v>
-      </c>
-      <c r="H59" t="s">
-        <v>399</v>
-      </c>
-      <c r="I59" t="s">
-        <v>400</v>
-      </c>
-      <c r="J59" t="s">
-        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>